<commit_message>
Remove incomplete & missing values
</commit_message>
<xml_diff>
--- a/data/raw/initial-attraction-online.xlsx
+++ b/data/raw/initial-attraction-online.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8ba3f9f5727e9d75/Projects/Hierarchy of Desire/R/hierarchy-desire/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaakk\OneDrive\Projects\Hierarchy of Desire\R\hierarchy-desire\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{216374DB-C789-42B8-A9A1-04FEBFB11E8F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{BD98C2B8-38D5-405A-89C3-6265C7655D2E}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{216374DB-C789-42B8-A9A1-04FEBFB11E8F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{7085BD42-0B13-4B04-9565-989F7D821E13}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8" windowWidth="23932" windowHeight="8370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -382,7 +382,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,6 +393,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEAEAE8"/>
         <bgColor rgb="FFEAEAE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -423,10 +429,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DG397"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I331" sqref="I331"/>
+    <sheetView tabSelected="1" topLeftCell="BM388" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BS20" activeCellId="38" sqref="BS392 BS380 BS376 BS367 BS358 BS350 BS347 BS315 BS314 BS313 BS311 BS293 BS286 BS285 BS280 BS262 BS248 BS228 BS223 BS207 BS200 BS197 BS196 BS191 BS188 BS160 BS129 BS122 BS102 BS91 BS86 BS54 BS51 BS48 BS31 BS30 BS23 BS21 BS20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4098,6 +4105,7 @@
       <c r="M20" t="s">
         <v>90</v>
       </c>
+      <c r="BS20" s="3"/>
     </row>
     <row r="21" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A21">
@@ -4181,6 +4189,7 @@
       <c r="BI21" t="s">
         <v>73</v>
       </c>
+      <c r="BS21" s="3"/>
     </row>
     <row r="22" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A22">
@@ -4353,6 +4362,7 @@
       <c r="I23" t="s">
         <v>63</v>
       </c>
+      <c r="BS23" s="3"/>
     </row>
     <row r="24" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A24">
@@ -5297,6 +5307,7 @@
       <c r="I30" t="s">
         <v>63</v>
       </c>
+      <c r="BS30" s="3"/>
     </row>
     <row r="31" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A31">
@@ -5335,6 +5346,7 @@
       <c r="AD31" t="s">
         <v>36</v>
       </c>
+      <c r="BS31" s="3"/>
     </row>
     <row r="32" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A32">
@@ -7997,6 +8009,7 @@
       <c r="BI48" t="s">
         <v>76</v>
       </c>
+      <c r="BS48" s="3"/>
     </row>
     <row r="49" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A49">
@@ -8369,6 +8382,7 @@
       <c r="I51" t="s">
         <v>63</v>
       </c>
+      <c r="BS51" s="3"/>
     </row>
     <row r="52" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A52">
@@ -8723,6 +8737,7 @@
       <c r="M54" t="s">
         <v>67</v>
       </c>
+      <c r="BS54" s="3"/>
     </row>
     <row r="55" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A55">
@@ -13701,6 +13716,7 @@
       <c r="AX86" t="s">
         <v>51</v>
       </c>
+      <c r="BS86" s="3"/>
     </row>
     <row r="87" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A87">
@@ -14371,6 +14387,7 @@
       <c r="I91" t="s">
         <v>63</v>
       </c>
+      <c r="BS91" s="3"/>
     </row>
     <row r="92" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A92">
@@ -15860,6 +15877,7 @@
       <c r="AT102" t="s">
         <v>47</v>
       </c>
+      <c r="BS102" s="3"/>
     </row>
     <row r="103" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A103">
@@ -19227,6 +19245,7 @@
       <c r="AM122" t="s">
         <v>45</v>
       </c>
+      <c r="BS122" s="3"/>
     </row>
     <row r="123" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A123">
@@ -20138,6 +20157,7 @@
       <c r="I129" t="s">
         <v>63</v>
       </c>
+      <c r="BS129" s="3"/>
     </row>
     <row r="130" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A130">
@@ -24949,6 +24969,7 @@
       <c r="M160" t="s">
         <v>67</v>
       </c>
+      <c r="BS160" s="3"/>
     </row>
     <row r="161" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A161">
@@ -29295,6 +29316,7 @@
       <c r="AL188" t="s">
         <v>44</v>
       </c>
+      <c r="BS188" s="3"/>
     </row>
     <row r="189" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A189">
@@ -29652,6 +29674,7 @@
       <c r="M191" t="s">
         <v>67</v>
       </c>
+      <c r="BS191" s="3"/>
     </row>
     <row r="192" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A192">
@@ -30223,6 +30246,7 @@
       <c r="M196" t="s">
         <v>77</v>
       </c>
+      <c r="BS196" s="3"/>
     </row>
     <row r="197" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A197">
@@ -30240,6 +30264,7 @@
       <c r="I197" t="s">
         <v>63</v>
       </c>
+      <c r="BS197" s="3"/>
     </row>
     <row r="198" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A198">
@@ -30594,6 +30619,7 @@
       <c r="I200" t="s">
         <v>63</v>
       </c>
+      <c r="BS200" s="3"/>
     </row>
     <row r="201" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A201">
@@ -31592,6 +31618,7 @@
       <c r="AD207" t="s">
         <v>36</v>
       </c>
+      <c r="BS207" s="3"/>
     </row>
     <row r="208" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A208">
@@ -34012,6 +34039,7 @@
       <c r="I223" t="s">
         <v>63</v>
       </c>
+      <c r="BS223" s="3"/>
     </row>
     <row r="224" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A224">
@@ -34760,6 +34788,7 @@
       <c r="AU228" t="s">
         <v>48</v>
       </c>
+      <c r="BS228" s="3"/>
     </row>
     <row r="229" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A229">
@@ -37800,6 +37829,7 @@
       <c r="AD248" t="s">
         <v>36</v>
       </c>
+      <c r="BS248" s="3"/>
     </row>
     <row r="249" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A249">
@@ -39853,6 +39883,7 @@
       <c r="AL262" t="s">
         <v>44</v>
       </c>
+      <c r="BS262" s="3"/>
     </row>
     <row r="263" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A263">
@@ -42619,6 +42650,7 @@
       <c r="AU280" t="s">
         <v>48</v>
       </c>
+      <c r="BS280" s="3"/>
     </row>
     <row r="281" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A281">
@@ -43340,6 +43372,7 @@
       <c r="AJ285" t="s">
         <v>42</v>
       </c>
+      <c r="BS285" s="3"/>
     </row>
     <row r="286" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A286">
@@ -43399,6 +43432,7 @@
       <c r="AY286" t="s">
         <v>52</v>
       </c>
+      <c r="BS286" s="3"/>
     </row>
     <row r="287" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A287">
@@ -44466,6 +44500,7 @@
       <c r="BI293" t="s">
         <v>73</v>
       </c>
+      <c r="BS293" s="3"/>
     </row>
     <row r="294" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A294">
@@ -47265,6 +47300,7 @@
       <c r="BI311" t="s">
         <v>72</v>
       </c>
+      <c r="BS311" s="3"/>
     </row>
     <row r="312" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A312">
@@ -47515,6 +47551,7 @@
       <c r="AX313" t="s">
         <v>51</v>
       </c>
+      <c r="BS313" s="3"/>
     </row>
     <row r="314" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A314">
@@ -47532,6 +47569,7 @@
       <c r="I314" t="s">
         <v>63</v>
       </c>
+      <c r="BS314" s="3"/>
     </row>
     <row r="315" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A315">
@@ -47594,6 +47632,7 @@
       <c r="AX315" t="s">
         <v>51</v>
       </c>
+      <c r="BS315" s="3"/>
     </row>
     <row r="316" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A316">
@@ -52431,6 +52470,7 @@
       <c r="I347" t="s">
         <v>63</v>
       </c>
+      <c r="BS347" s="3"/>
     </row>
     <row r="348" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A348">
@@ -52818,6 +52858,7 @@
       <c r="AM350" t="s">
         <v>45</v>
       </c>
+      <c r="BS350" s="3"/>
     </row>
     <row r="351" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A351">
@@ -53986,6 +54027,7 @@
       <c r="BI358" t="s">
         <v>72</v>
       </c>
+      <c r="BS358" s="3"/>
     </row>
     <row r="359" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A359">
@@ -55387,6 +55429,7 @@
       <c r="AJ367" t="s">
         <v>42</v>
       </c>
+      <c r="BS367" s="3"/>
     </row>
     <row r="368" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A368">
@@ -56773,6 +56816,7 @@
       <c r="BN376" t="s">
         <v>53</v>
       </c>
+      <c r="BS376" s="3"/>
     </row>
     <row r="377" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A377">
@@ -57318,6 +57362,7 @@
       <c r="AX380" t="s">
         <v>51</v>
       </c>
+      <c r="BS380" s="3"/>
     </row>
     <row r="381" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A381">
@@ -59187,6 +59232,7 @@
       <c r="I392" t="s">
         <v>63</v>
       </c>
+      <c r="BS392" s="3"/>
     </row>
     <row r="393" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A393">

</xml_diff>